<commit_message>
Reading files and mapping working.
</commit_message>
<xml_diff>
--- a/datasets/20161003 pJP22mcherry 01.xlsx
+++ b/datasets/20161003 pJP22mcherry 01.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thmosqueiro/Desktop/igem2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thmosqueiro/Desktop/igem2017/modeliGEM2016/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="final" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>

</xml_diff>